<commit_message>
Answered some basic questions on chesstempo puzzles
</commit_message>
<xml_diff>
--- a/data/input/chesstempo_tactics.xlsx
+++ b/data/input/chesstempo_tactics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Desktop\chess\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Desktop\chess\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="878">
   <si>
     <t>969.4</t>
   </si>
@@ -2337,6 +2337,327 @@
   </si>
   <si>
     <t>1385.3 (+9.7)</t>
+  </si>
+  <si>
+    <t>1360.8</t>
+  </si>
+  <si>
+    <t>1371.1 (-3.6)</t>
+  </si>
+  <si>
+    <t>1263.2</t>
+  </si>
+  <si>
+    <t>1374.7 (+2.4)</t>
+  </si>
+  <si>
+    <t>1405.1</t>
+  </si>
+  <si>
+    <t>1372.3 (-3.2)</t>
+  </si>
+  <si>
+    <t>1491.3</t>
+  </si>
+  <si>
+    <t>1375.5 (+4.7)</t>
+  </si>
+  <si>
+    <t>1221.9</t>
+  </si>
+  <si>
+    <t>1370.8 (+2.1)</t>
+  </si>
+  <si>
+    <t>1502.3</t>
+  </si>
+  <si>
+    <t>1368.7 (+4.8)</t>
+  </si>
+  <si>
+    <t>1363.9 (+2.6)</t>
+  </si>
+  <si>
+    <t>1242.8</t>
+  </si>
+  <si>
+    <t>1361.3 (-4.7)</t>
+  </si>
+  <si>
+    <t>1310.0</t>
+  </si>
+  <si>
+    <t>1365.9 (-4.1)</t>
+  </si>
+  <si>
+    <t>1428.7</t>
+  </si>
+  <si>
+    <t>1370.0 (+4.1)</t>
+  </si>
+  <si>
+    <t>1194.4</t>
+  </si>
+  <si>
+    <t>1365.9 (+1.9)</t>
+  </si>
+  <si>
+    <t>1404.0</t>
+  </si>
+  <si>
+    <t>1364.0 (-3.1)</t>
+  </si>
+  <si>
+    <t>1339.5</t>
+  </si>
+  <si>
+    <t>1367.1 (-3.8)</t>
+  </si>
+  <si>
+    <t>1325.6</t>
+  </si>
+  <si>
+    <t>1370.9 (-4.0)</t>
+  </si>
+  <si>
+    <t>1363.4</t>
+  </si>
+  <si>
+    <t>1374.9 (+3.4)</t>
+  </si>
+  <si>
+    <t>1292.9</t>
+  </si>
+  <si>
+    <t>1371.5 (-4.5)</t>
+  </si>
+  <si>
+    <t>1261.4</t>
+  </si>
+  <si>
+    <t>1376.0 (+2.6)</t>
+  </si>
+  <si>
+    <t>1221.4</t>
+  </si>
+  <si>
+    <t>1373.4 (-5.6)</t>
+  </si>
+  <si>
+    <t>1238.9</t>
+  </si>
+  <si>
+    <t>1379.0 (+2.6)</t>
+  </si>
+  <si>
+    <t>1229.2</t>
+  </si>
+  <si>
+    <t>1391.1 (+2.0)</t>
+  </si>
+  <si>
+    <t>1240.3</t>
+  </si>
+  <si>
+    <t>1389.1 (+2.1)</t>
+  </si>
+  <si>
+    <t>1311.4</t>
+  </si>
+  <si>
+    <t>1387.0 (+2.8)</t>
+  </si>
+  <si>
+    <t>1151.5</t>
+  </si>
+  <si>
+    <t>1384.2 (+1.5)</t>
+  </si>
+  <si>
+    <t>1277.9</t>
+  </si>
+  <si>
+    <t>1382.8 (+2.5)</t>
+  </si>
+  <si>
+    <t>1384.4</t>
+  </si>
+  <si>
+    <t>1380.3 (+3.6)</t>
+  </si>
+  <si>
+    <t>1601.0</t>
+  </si>
+  <si>
+    <t>1376.7 (-1.5)</t>
+  </si>
+  <si>
+    <t>1185.9</t>
+  </si>
+  <si>
+    <t>1378.2 (+1.8)</t>
+  </si>
+  <si>
+    <t>996.1</t>
+  </si>
+  <si>
+    <t>1376.5 (+0.7)</t>
+  </si>
+  <si>
+    <t>1513.6</t>
+  </si>
+  <si>
+    <t>1375.8 (+4.9)</t>
+  </si>
+  <si>
+    <t>1370.9 (-4.9)</t>
+  </si>
+  <si>
+    <t>1197.8</t>
+  </si>
+  <si>
+    <t>1375.9 (+1.9)</t>
+  </si>
+  <si>
+    <t>1303.0</t>
+  </si>
+  <si>
+    <t>1374.0 (+2.9)</t>
+  </si>
+  <si>
+    <t>1384.0 (+2.1)</t>
+  </si>
+  <si>
+    <t>1267.5</t>
+  </si>
+  <si>
+    <t>1381.9 (-4.6)</t>
+  </si>
+  <si>
+    <t>1341.6</t>
+  </si>
+  <si>
+    <t>1386.6 (-4.0)</t>
+  </si>
+  <si>
+    <t>1275.7</t>
+  </si>
+  <si>
+    <t>1390.6 (+2.4)</t>
+  </si>
+  <si>
+    <t>1102.1</t>
+  </si>
+  <si>
+    <t>1388.2 (+1.1)</t>
+  </si>
+  <si>
+    <t>1201.7</t>
+  </si>
+  <si>
+    <t>1387.0 (+1.8)</t>
+  </si>
+  <si>
+    <t>1333.2</t>
+  </si>
+  <si>
+    <t>1385.2 (+3.0)</t>
+  </si>
+  <si>
+    <t>1347.1</t>
+  </si>
+  <si>
+    <t>1382.2 (-3.9)</t>
+  </si>
+  <si>
+    <t>1195.3</t>
+  </si>
+  <si>
+    <t>1386.1 (-5.3)</t>
+  </si>
+  <si>
+    <t>1314.9</t>
+  </si>
+  <si>
+    <t>1391.4 (-4.3)</t>
+  </si>
+  <si>
+    <t>1237.0</t>
+  </si>
+  <si>
+    <t>1395.7 (-5.0)</t>
+  </si>
+  <si>
+    <t>1211.9</t>
+  </si>
+  <si>
+    <t>1400.7 (+1.8)</t>
+  </si>
+  <si>
+    <t>1131.9</t>
+  </si>
+  <si>
+    <t>1398.9 (+1.2)</t>
+  </si>
+  <si>
+    <t>1239.0</t>
+  </si>
+  <si>
+    <t>1397.6 (+2.0)</t>
+  </si>
+  <si>
+    <t>1395.6 (+1.4)</t>
+  </si>
+  <si>
+    <t>1259.3</t>
+  </si>
+  <si>
+    <t>1394.2 (+2.2)</t>
+  </si>
+  <si>
+    <t>1217.2</t>
+  </si>
+  <si>
+    <t>1392.0 (+1.9)</t>
+  </si>
+  <si>
+    <t>1155.1</t>
+  </si>
+  <si>
+    <t>1390.1 (+1.4)</t>
+  </si>
+  <si>
+    <t>1152.4</t>
+  </si>
+  <si>
+    <t>1388.7 (+1.4)</t>
+  </si>
+  <si>
+    <t>1427.9</t>
+  </si>
+  <si>
+    <t>1387.2 (-3.1)</t>
+  </si>
+  <si>
+    <t>1390.3 (+2.3)</t>
+  </si>
+  <si>
+    <t>1355.6</t>
+  </si>
+  <si>
+    <t>1388.1 (+3.2)</t>
+  </si>
+  <si>
+    <t>1382.5</t>
+  </si>
+  <si>
+    <t>1384.9 (-3.5)</t>
+  </si>
+  <si>
+    <t>1472.0</t>
+  </si>
+  <si>
+    <t>1388.4 (-2.7)</t>
   </si>
 </sst>
 </file>
@@ -2656,10 +2977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I394"/>
+  <dimension ref="A1:I450"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
-      <selection activeCell="B376" sqref="B376"/>
+    <sheetView tabSelected="1" topLeftCell="A410" workbookViewId="0">
+      <selection activeCell="A427" sqref="A427:I450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14093,6 +14414,1630 @@
         <v>770</v>
       </c>
     </row>
+    <row r="395" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>1</v>
+      </c>
+      <c r="B395" s="1">
+        <v>42750.916122685187</v>
+      </c>
+      <c r="C395">
+        <v>54001</v>
+      </c>
+      <c r="D395" t="s">
+        <v>771</v>
+      </c>
+      <c r="E395" t="s">
+        <v>1</v>
+      </c>
+      <c r="F395" s="2">
+        <v>0.12361111111111112</v>
+      </c>
+      <c r="G395" s="2">
+        <v>0.11388888888888889</v>
+      </c>
+      <c r="H395" s="2">
+        <v>0</v>
+      </c>
+      <c r="I395" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="396" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>2</v>
+      </c>
+      <c r="B396" s="1">
+        <v>42750.914178240739</v>
+      </c>
+      <c r="C396">
+        <v>152611</v>
+      </c>
+      <c r="D396" t="s">
+        <v>773</v>
+      </c>
+      <c r="E396" t="s">
+        <v>1</v>
+      </c>
+      <c r="F396" s="2">
+        <v>4.027777777777778E-2</v>
+      </c>
+      <c r="G396" s="2">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H396" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I396" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="397" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>3</v>
+      </c>
+      <c r="B397" s="1">
+        <v>42750.913703703707</v>
+      </c>
+      <c r="C397">
+        <v>180933</v>
+      </c>
+      <c r="D397" t="s">
+        <v>775</v>
+      </c>
+      <c r="E397" t="s">
+        <v>1</v>
+      </c>
+      <c r="F397" s="2">
+        <v>6.458333333333334E-2</v>
+      </c>
+      <c r="G397" s="2">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="H397" s="2">
+        <v>0</v>
+      </c>
+      <c r="I397" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="398" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>4</v>
+      </c>
+      <c r="B398" s="1">
+        <v>42750.913136574076</v>
+      </c>
+      <c r="C398">
+        <v>171450</v>
+      </c>
+      <c r="D398" t="s">
+        <v>777</v>
+      </c>
+      <c r="E398" t="s">
+        <v>1</v>
+      </c>
+      <c r="F398" s="2">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="G398" s="2">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="H398" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I398" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="399" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>5</v>
+      </c>
+      <c r="B399" s="1">
+        <v>42750.912245370368</v>
+      </c>
+      <c r="C399">
+        <v>126789</v>
+      </c>
+      <c r="D399" t="s">
+        <v>779</v>
+      </c>
+      <c r="E399" t="s">
+        <v>1</v>
+      </c>
+      <c r="F399" s="2">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="G399" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H399" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I399" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="400" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>6</v>
+      </c>
+      <c r="B400" s="1">
+        <v>42750.911678240744</v>
+      </c>
+      <c r="C400">
+        <v>47655</v>
+      </c>
+      <c r="D400" t="s">
+        <v>781</v>
+      </c>
+      <c r="E400" t="s">
+        <v>1</v>
+      </c>
+      <c r="F400" s="2">
+        <v>9.2361111111111116E-2</v>
+      </c>
+      <c r="G400" s="2">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="H400" s="2">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="I400" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="401" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>7</v>
+      </c>
+      <c r="B401" s="1">
+        <v>42750.910844907405</v>
+      </c>
+      <c r="C401">
+        <v>4425</v>
+      </c>
+      <c r="D401" t="s">
+        <v>585</v>
+      </c>
+      <c r="E401" t="s">
+        <v>1</v>
+      </c>
+      <c r="F401" s="2">
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="G401" s="2">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H401" s="2">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="I401" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="402" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>8</v>
+      </c>
+      <c r="B402" s="1">
+        <v>42750.909953703704</v>
+      </c>
+      <c r="C402">
+        <v>160057</v>
+      </c>
+      <c r="D402" t="s">
+        <v>784</v>
+      </c>
+      <c r="E402" t="s">
+        <v>1</v>
+      </c>
+      <c r="F402" s="2">
+        <v>0.14166666666666666</v>
+      </c>
+      <c r="G402" s="2">
+        <v>0.11875000000000001</v>
+      </c>
+      <c r="H402" s="2">
+        <v>0</v>
+      </c>
+      <c r="I402" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="403" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>9</v>
+      </c>
+      <c r="B403" s="1">
+        <v>42750.907870370371</v>
+      </c>
+      <c r="C403">
+        <v>63624</v>
+      </c>
+      <c r="D403" t="s">
+        <v>786</v>
+      </c>
+      <c r="E403" t="s">
+        <v>1</v>
+      </c>
+      <c r="F403" s="2">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="G403" s="2">
+        <v>8.0555555555555561E-2</v>
+      </c>
+      <c r="H403" s="2">
+        <v>0</v>
+      </c>
+      <c r="I403" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="404" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>10</v>
+      </c>
+      <c r="B404" s="1">
+        <v>42750.905995370369</v>
+      </c>
+      <c r="C404">
+        <v>139884</v>
+      </c>
+      <c r="D404" t="s">
+        <v>788</v>
+      </c>
+      <c r="E404" t="s">
+        <v>1</v>
+      </c>
+      <c r="F404" s="2">
+        <v>0.10277777777777779</v>
+      </c>
+      <c r="G404" s="2">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="H404" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I404" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="405" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>11</v>
+      </c>
+      <c r="B405" s="1">
+        <v>42750.905069444445</v>
+      </c>
+      <c r="C405">
+        <v>144650</v>
+      </c>
+      <c r="D405" t="s">
+        <v>790</v>
+      </c>
+      <c r="E405" t="s">
+        <v>1</v>
+      </c>
+      <c r="F405" s="2">
+        <v>9.4444444444444442E-2</v>
+      </c>
+      <c r="G405" s="2">
+        <v>5.347222222222222E-2</v>
+      </c>
+      <c r="H405" s="2">
+        <v>2.8472222222222222E-2</v>
+      </c>
+      <c r="I405" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="406" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>12</v>
+      </c>
+      <c r="B406" s="1">
+        <v>42750.903958333336</v>
+      </c>
+      <c r="C406">
+        <v>71089</v>
+      </c>
+      <c r="D406" t="s">
+        <v>792</v>
+      </c>
+      <c r="E406" t="s">
+        <v>1</v>
+      </c>
+      <c r="F406" s="2">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G406" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H406" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I406" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="407" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>13</v>
+      </c>
+      <c r="B407" s="1">
+        <v>42750.903622685182</v>
+      </c>
+      <c r="C407">
+        <v>64811</v>
+      </c>
+      <c r="D407" t="s">
+        <v>794</v>
+      </c>
+      <c r="E407" t="s">
+        <v>1</v>
+      </c>
+      <c r="F407" s="2">
+        <v>6.1805555555555558E-2</v>
+      </c>
+      <c r="G407" s="2">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="H407" s="2">
+        <v>0</v>
+      </c>
+      <c r="I407" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="408" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>14</v>
+      </c>
+      <c r="B408" s="1">
+        <v>42750.902384259258</v>
+      </c>
+      <c r="C408">
+        <v>103367</v>
+      </c>
+      <c r="D408" t="s">
+        <v>796</v>
+      </c>
+      <c r="E408" t="s">
+        <v>1</v>
+      </c>
+      <c r="F408" s="2">
+        <v>7.8472222222222221E-2</v>
+      </c>
+      <c r="G408" s="2">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="H408" s="2">
+        <v>0</v>
+      </c>
+      <c r="I408" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="409" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>15</v>
+      </c>
+      <c r="B409" s="1">
+        <v>42750.901956018519</v>
+      </c>
+      <c r="C409">
+        <v>120738</v>
+      </c>
+      <c r="D409" t="s">
+        <v>798</v>
+      </c>
+      <c r="E409" t="s">
+        <v>1</v>
+      </c>
+      <c r="F409" s="2">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="G409" s="2">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="H409" s="2">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="I409" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="410" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>16</v>
+      </c>
+      <c r="B410" s="1">
+        <v>42750.900868055556</v>
+      </c>
+      <c r="C410">
+        <v>97570</v>
+      </c>
+      <c r="D410" t="s">
+        <v>800</v>
+      </c>
+      <c r="E410" t="s">
+        <v>1</v>
+      </c>
+      <c r="F410" s="2">
+        <v>0.11180555555555556</v>
+      </c>
+      <c r="G410" s="2">
+        <v>7.9166666666666663E-2</v>
+      </c>
+      <c r="H410" s="2">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="I410" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="411" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>17</v>
+      </c>
+      <c r="B411" s="1">
+        <v>42750.897210648145</v>
+      </c>
+      <c r="C411">
+        <v>32443</v>
+      </c>
+      <c r="D411" t="s">
+        <v>802</v>
+      </c>
+      <c r="E411" t="s">
+        <v>1</v>
+      </c>
+      <c r="F411" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="G411" s="2">
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="H411" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I411" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="412" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>18</v>
+      </c>
+      <c r="B412" s="1">
+        <v>42750.895868055559</v>
+      </c>
+      <c r="C412">
+        <v>71605</v>
+      </c>
+      <c r="D412" t="s">
+        <v>804</v>
+      </c>
+      <c r="E412" t="s">
+        <v>1</v>
+      </c>
+      <c r="F412" s="2">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="G412" s="2">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="H412" s="2">
+        <v>0</v>
+      </c>
+      <c r="I412" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="413" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>19</v>
+      </c>
+      <c r="B413" s="1">
+        <v>42750.89539351852</v>
+      </c>
+      <c r="C413">
+        <v>77726</v>
+      </c>
+      <c r="D413" t="s">
+        <v>806</v>
+      </c>
+      <c r="E413" t="s">
+        <v>1</v>
+      </c>
+      <c r="F413" s="2">
+        <v>9.3055555555555558E-2</v>
+      </c>
+      <c r="G413" s="2">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="H413" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="I413" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="414" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>1</v>
+      </c>
+      <c r="B414" s="1">
+        <v>42751.577372685184</v>
+      </c>
+      <c r="C414">
+        <v>79249</v>
+      </c>
+      <c r="D414" t="s">
+        <v>808</v>
+      </c>
+      <c r="E414" t="s">
+        <v>1</v>
+      </c>
+      <c r="F414" s="2">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="G414" s="2">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="H414" s="2">
+        <v>0</v>
+      </c>
+      <c r="I414" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="415" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>2</v>
+      </c>
+      <c r="B415" s="1">
+        <v>42751.577118055553</v>
+      </c>
+      <c r="C415">
+        <v>163534</v>
+      </c>
+      <c r="D415" t="s">
+        <v>810</v>
+      </c>
+      <c r="E415" t="s">
+        <v>1</v>
+      </c>
+      <c r="F415" s="2">
+        <v>6.5277777777777782E-2</v>
+      </c>
+      <c r="G415" s="2">
+        <v>1.5277777777777777E-2</v>
+      </c>
+      <c r="H415" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="I415" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="416" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>3</v>
+      </c>
+      <c r="B416" s="1">
+        <v>42751.57675925926</v>
+      </c>
+      <c r="C416">
+        <v>156601</v>
+      </c>
+      <c r="D416" t="s">
+        <v>812</v>
+      </c>
+      <c r="E416" t="s">
+        <v>1</v>
+      </c>
+      <c r="F416" s="2">
+        <v>6.3194444444444442E-2</v>
+      </c>
+      <c r="G416" s="2">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="H416" s="2">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="I416" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="417" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>4</v>
+      </c>
+      <c r="B417" s="1">
+        <v>42751.576377314814</v>
+      </c>
+      <c r="C417">
+        <v>54052</v>
+      </c>
+      <c r="D417" t="s">
+        <v>814</v>
+      </c>
+      <c r="E417" t="s">
+        <v>1</v>
+      </c>
+      <c r="F417" s="2">
+        <v>3.5416666666666666E-2</v>
+      </c>
+      <c r="G417" s="2">
+        <v>7.8472222222222221E-2</v>
+      </c>
+      <c r="H417" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="I417" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="418" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>5</v>
+      </c>
+      <c r="B418" s="1">
+        <v>42751.575046296297</v>
+      </c>
+      <c r="C418">
+        <v>31474</v>
+      </c>
+      <c r="D418" t="s">
+        <v>816</v>
+      </c>
+      <c r="E418" t="s">
+        <v>1</v>
+      </c>
+      <c r="F418" s="2">
+        <v>7.3611111111111113E-2</v>
+      </c>
+      <c r="G418" s="2">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="H418" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I418" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="419" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>6</v>
+      </c>
+      <c r="B419" s="1">
+        <v>42751.565648148149</v>
+      </c>
+      <c r="C419">
+        <v>65343</v>
+      </c>
+      <c r="D419" t="s">
+        <v>818</v>
+      </c>
+      <c r="E419" t="s">
+        <v>1</v>
+      </c>
+      <c r="F419" s="2">
+        <v>0.10555555555555556</v>
+      </c>
+      <c r="G419" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="H419" s="2">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="I419" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="420" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>7</v>
+      </c>
+      <c r="B420" s="1">
+        <v>42751.564756944441</v>
+      </c>
+      <c r="C420">
+        <v>109727</v>
+      </c>
+      <c r="D420" t="s">
+        <v>820</v>
+      </c>
+      <c r="E420" t="s">
+        <v>1</v>
+      </c>
+      <c r="F420" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="G420" s="2">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="H420" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="I420" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="421" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>8</v>
+      </c>
+      <c r="B421" s="1">
+        <v>42751.56391203704</v>
+      </c>
+      <c r="C421">
+        <v>171100</v>
+      </c>
+      <c r="D421" t="s">
+        <v>822</v>
+      </c>
+      <c r="E421" t="s">
+        <v>1</v>
+      </c>
+      <c r="F421" s="2">
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="G421" s="2">
+        <v>7.1527777777777787E-2</v>
+      </c>
+      <c r="H421" s="2">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="I421" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="422" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>9</v>
+      </c>
+      <c r="B422" s="1">
+        <v>42751.562673611108</v>
+      </c>
+      <c r="C422">
+        <v>53049</v>
+      </c>
+      <c r="D422" t="s">
+        <v>824</v>
+      </c>
+      <c r="E422" t="s">
+        <v>1</v>
+      </c>
+      <c r="F422" s="2">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="G422" s="2">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="H422" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I422" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="423" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>10</v>
+      </c>
+      <c r="B423" s="1">
+        <v>42751.562442129631</v>
+      </c>
+      <c r="C423">
+        <v>45697</v>
+      </c>
+      <c r="D423" t="s">
+        <v>826</v>
+      </c>
+      <c r="E423" t="s">
+        <v>1</v>
+      </c>
+      <c r="F423" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G423" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="H423" s="2">
+        <v>0</v>
+      </c>
+      <c r="I423" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="424" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A424">
+        <v>11</v>
+      </c>
+      <c r="B424" s="1">
+        <v>42751.562164351853</v>
+      </c>
+      <c r="C424">
+        <v>104460</v>
+      </c>
+      <c r="D424" t="s">
+        <v>390</v>
+      </c>
+      <c r="E424" t="s">
+        <v>1</v>
+      </c>
+      <c r="F424" s="2">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="G424" s="2">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="H424" s="2">
+        <v>0</v>
+      </c>
+      <c r="I424" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="425" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>12</v>
+      </c>
+      <c r="B425" s="1">
+        <v>42751.560914351852</v>
+      </c>
+      <c r="C425">
+        <v>40376</v>
+      </c>
+      <c r="D425" t="s">
+        <v>829</v>
+      </c>
+      <c r="E425" t="s">
+        <v>1</v>
+      </c>
+      <c r="F425" s="2">
+        <v>3.4027777777777775E-2</v>
+      </c>
+      <c r="G425" s="2">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="H425" s="2">
+        <v>0</v>
+      </c>
+      <c r="I425" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="426" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>13</v>
+      </c>
+      <c r="B426" s="1">
+        <v>42751.560752314814</v>
+      </c>
+      <c r="C426">
+        <v>96805</v>
+      </c>
+      <c r="D426" t="s">
+        <v>831</v>
+      </c>
+      <c r="E426" t="s">
+        <v>1</v>
+      </c>
+      <c r="F426" s="2">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="G426" s="2">
+        <v>1.8055555555555557E-2</v>
+      </c>
+      <c r="H426" s="2">
+        <v>0</v>
+      </c>
+      <c r="I426" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="427" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A427">
+        <v>1</v>
+      </c>
+      <c r="B427" s="1">
+        <v>42751.74800925926</v>
+      </c>
+      <c r="C427">
+        <v>62966</v>
+      </c>
+      <c r="D427" t="s">
+        <v>618</v>
+      </c>
+      <c r="E427" t="s">
+        <v>1</v>
+      </c>
+      <c r="F427" s="2">
+        <v>6.1805555555555558E-2</v>
+      </c>
+      <c r="G427" s="2">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="H427" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I427" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="428" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A428">
+        <v>2</v>
+      </c>
+      <c r="B428" s="1">
+        <v>42751.745370370372</v>
+      </c>
+      <c r="C428">
+        <v>91661</v>
+      </c>
+      <c r="D428" t="s">
+        <v>834</v>
+      </c>
+      <c r="E428" t="s">
+        <v>1</v>
+      </c>
+      <c r="F428" s="2">
+        <v>0.10902777777777778</v>
+      </c>
+      <c r="G428" s="2">
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="H428" s="2">
+        <v>0</v>
+      </c>
+      <c r="I428" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="429" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A429">
+        <v>3</v>
+      </c>
+      <c r="B429" s="1">
+        <v>42751.743819444448</v>
+      </c>
+      <c r="C429">
+        <v>170802</v>
+      </c>
+      <c r="D429" t="s">
+        <v>836</v>
+      </c>
+      <c r="E429" t="s">
+        <v>1</v>
+      </c>
+      <c r="F429" s="2">
+        <v>7.7083333333333337E-2</v>
+      </c>
+      <c r="G429" s="2">
+        <v>5.6250000000000001E-2</v>
+      </c>
+      <c r="H429" s="2">
+        <v>0</v>
+      </c>
+      <c r="I429" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="430" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>4</v>
+      </c>
+      <c r="B430" s="1">
+        <v>42751.742847222224</v>
+      </c>
+      <c r="C430">
+        <v>75685</v>
+      </c>
+      <c r="D430" t="s">
+        <v>838</v>
+      </c>
+      <c r="E430" t="s">
+        <v>1</v>
+      </c>
+      <c r="F430" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="G430" s="2">
+        <v>6.1111111111111116E-2</v>
+      </c>
+      <c r="H430" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="I430" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="431" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>5</v>
+      </c>
+      <c r="B431" s="1">
+        <v>42751.741782407407</v>
+      </c>
+      <c r="C431">
+        <v>87760</v>
+      </c>
+      <c r="D431" t="s">
+        <v>840</v>
+      </c>
+      <c r="E431" t="s">
+        <v>1</v>
+      </c>
+      <c r="F431" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G431" s="2">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="H431" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I431" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="432" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A432">
+        <v>6</v>
+      </c>
+      <c r="B432" s="1">
+        <v>42751.741620370369</v>
+      </c>
+      <c r="C432">
+        <v>260</v>
+      </c>
+      <c r="D432" t="s">
+        <v>842</v>
+      </c>
+      <c r="E432" t="s">
+        <v>1</v>
+      </c>
+      <c r="F432" s="2">
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="G432" s="2">
+        <v>1.8055555555555557E-2</v>
+      </c>
+      <c r="H432" s="2">
+        <v>0</v>
+      </c>
+      <c r="I432" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="433" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>7</v>
+      </c>
+      <c r="B433" s="1">
+        <v>42751.741284722222</v>
+      </c>
+      <c r="C433">
+        <v>165499</v>
+      </c>
+      <c r="D433" t="s">
+        <v>844</v>
+      </c>
+      <c r="E433" t="s">
+        <v>1</v>
+      </c>
+      <c r="F433" s="2">
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="G433" s="2">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="H433" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I433" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="434" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A434">
+        <v>8</v>
+      </c>
+      <c r="B434" s="1">
+        <v>42751.740763888891</v>
+      </c>
+      <c r="C434">
+        <v>53889</v>
+      </c>
+      <c r="D434" t="s">
+        <v>846</v>
+      </c>
+      <c r="E434" t="s">
+        <v>1</v>
+      </c>
+      <c r="F434" s="2">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="G434" s="2">
+        <v>3.1944444444444449E-2</v>
+      </c>
+      <c r="H434" s="2">
+        <v>0</v>
+      </c>
+      <c r="I434" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="435" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A435">
+        <v>9</v>
+      </c>
+      <c r="B435" s="1">
+        <v>42751.74013888889</v>
+      </c>
+      <c r="C435">
+        <v>149676</v>
+      </c>
+      <c r="D435" t="s">
+        <v>848</v>
+      </c>
+      <c r="E435" t="s">
+        <v>1</v>
+      </c>
+      <c r="F435" s="2">
+        <v>3.5416666666666666E-2</v>
+      </c>
+      <c r="G435" s="2">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="H435" s="2">
+        <v>0</v>
+      </c>
+      <c r="I435" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="436" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A436">
+        <v>10</v>
+      </c>
+      <c r="B436" s="1">
+        <v>42751.739756944444</v>
+      </c>
+      <c r="C436">
+        <v>144849</v>
+      </c>
+      <c r="D436" t="s">
+        <v>850</v>
+      </c>
+      <c r="E436" t="s">
+        <v>1</v>
+      </c>
+      <c r="F436" s="2">
+        <v>0.13472222222222222</v>
+      </c>
+      <c r="G436" s="2">
+        <v>0.24861111111111112</v>
+      </c>
+      <c r="H436" s="2">
+        <v>0</v>
+      </c>
+      <c r="I436" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="437" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A437">
+        <v>11</v>
+      </c>
+      <c r="B437" s="1">
+        <v>42751.733634259261</v>
+      </c>
+      <c r="C437">
+        <v>178099</v>
+      </c>
+      <c r="D437" t="s">
+        <v>852</v>
+      </c>
+      <c r="E437" t="s">
+        <v>1</v>
+      </c>
+      <c r="F437" s="2">
+        <v>0.15138888888888888</v>
+      </c>
+      <c r="G437" s="2">
+        <v>3.5416666666666666E-2</v>
+      </c>
+      <c r="H437" s="2">
+        <v>0</v>
+      </c>
+      <c r="I437" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="438" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A438">
+        <v>12</v>
+      </c>
+      <c r="B438" s="1">
+        <v>42751.732986111114</v>
+      </c>
+      <c r="C438">
+        <v>43767</v>
+      </c>
+      <c r="D438" t="s">
+        <v>854</v>
+      </c>
+      <c r="E438" t="s">
+        <v>1</v>
+      </c>
+      <c r="F438" s="2">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="G438" s="2">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="H438" s="2">
+        <v>0</v>
+      </c>
+      <c r="I438" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="439" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A439">
+        <v>13</v>
+      </c>
+      <c r="B439" s="1">
+        <v>42751.732812499999</v>
+      </c>
+      <c r="C439">
+        <v>175740</v>
+      </c>
+      <c r="D439" t="s">
+        <v>856</v>
+      </c>
+      <c r="E439" t="s">
+        <v>1</v>
+      </c>
+      <c r="F439" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G439" s="2">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H439" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I439" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="440" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A440">
+        <v>14</v>
+      </c>
+      <c r="B440" s="1">
+        <v>42751.732499999998</v>
+      </c>
+      <c r="C440">
+        <v>179435</v>
+      </c>
+      <c r="D440" t="s">
+        <v>858</v>
+      </c>
+      <c r="E440" t="s">
+        <v>1</v>
+      </c>
+      <c r="F440" s="2">
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="G440" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H440" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I440" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="441" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A441">
+        <v>15</v>
+      </c>
+      <c r="B441" s="1">
+        <v>42751.732118055559</v>
+      </c>
+      <c r="C441">
+        <v>48017</v>
+      </c>
+      <c r="D441" t="s">
+        <v>814</v>
+      </c>
+      <c r="E441" t="s">
+        <v>1</v>
+      </c>
+      <c r="F441" s="2">
+        <v>6.1805555555555558E-2</v>
+      </c>
+      <c r="G441" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="H441" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I441" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="442" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A442">
+        <v>16</v>
+      </c>
+      <c r="B442" s="1">
+        <v>42751.73128472222</v>
+      </c>
+      <c r="C442">
+        <v>90300</v>
+      </c>
+      <c r="D442" t="s">
+        <v>861</v>
+      </c>
+      <c r="E442" t="s">
+        <v>1</v>
+      </c>
+      <c r="F442" s="2">
+        <v>2.5694444444444447E-2</v>
+      </c>
+      <c r="G442" s="2">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="H442" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I442" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="443" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A443">
+        <v>17</v>
+      </c>
+      <c r="B443" s="1">
+        <v>42751.730949074074</v>
+      </c>
+      <c r="C443">
+        <v>101201</v>
+      </c>
+      <c r="D443" t="s">
+        <v>863</v>
+      </c>
+      <c r="E443" t="s">
+        <v>1</v>
+      </c>
+      <c r="F443" s="2">
+        <v>6.5277777777777782E-2</v>
+      </c>
+      <c r="G443" s="2">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="H443" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I443" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="444" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A444">
+        <v>18</v>
+      </c>
+      <c r="B444" s="1">
+        <v>42751.730578703704</v>
+      </c>
+      <c r="C444">
+        <v>45739</v>
+      </c>
+      <c r="D444" t="s">
+        <v>865</v>
+      </c>
+      <c r="E444" t="s">
+        <v>1</v>
+      </c>
+      <c r="F444" s="2">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="G444" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H444" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I444" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="445" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A445">
+        <v>19</v>
+      </c>
+      <c r="B445" s="1">
+        <v>42751.730312500003</v>
+      </c>
+      <c r="C445">
+        <v>73590</v>
+      </c>
+      <c r="D445" t="s">
+        <v>867</v>
+      </c>
+      <c r="E445" t="s">
+        <v>1</v>
+      </c>
+      <c r="F445" s="2">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="G445" s="2">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="H445" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I445" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="446" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A446">
+        <v>20</v>
+      </c>
+      <c r="B446" s="1">
+        <v>42751.729270833333</v>
+      </c>
+      <c r="C446">
+        <v>91615</v>
+      </c>
+      <c r="D446" t="s">
+        <v>869</v>
+      </c>
+      <c r="E446" t="s">
+        <v>1</v>
+      </c>
+      <c r="F446" s="2">
+        <v>7.9166666666666663E-2</v>
+      </c>
+      <c r="G446" s="2">
+        <v>3.5416666666666666E-2</v>
+      </c>
+      <c r="H446" s="2">
+        <v>0</v>
+      </c>
+      <c r="I446" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="447" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A447">
+        <v>21</v>
+      </c>
+      <c r="B447" s="1">
+        <v>42751.72861111111</v>
+      </c>
+      <c r="C447">
+        <v>162860</v>
+      </c>
+      <c r="D447" t="s">
+        <v>756</v>
+      </c>
+      <c r="E447" t="s">
+        <v>1</v>
+      </c>
+      <c r="F447" s="2">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="G447" s="2">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="H447" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I447" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="448" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A448">
+        <v>22</v>
+      </c>
+      <c r="B448" s="1">
+        <v>42751.728356481479</v>
+      </c>
+      <c r="C448">
+        <v>163556</v>
+      </c>
+      <c r="D448" t="s">
+        <v>872</v>
+      </c>
+      <c r="E448" t="s">
+        <v>1</v>
+      </c>
+      <c r="F448" s="2">
+        <v>0.12013888888888889</v>
+      </c>
+      <c r="G448" s="2">
+        <v>0.10486111111111111</v>
+      </c>
+      <c r="H448" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I448" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="449" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>23</v>
+      </c>
+      <c r="B449" s="1">
+        <v>42751.726377314815</v>
+      </c>
+      <c r="C449">
+        <v>74865</v>
+      </c>
+      <c r="D449" t="s">
+        <v>874</v>
+      </c>
+      <c r="E449" t="s">
+        <v>1</v>
+      </c>
+      <c r="F449" s="2">
+        <v>5.8333333333333327E-2</v>
+      </c>
+      <c r="G449" s="2">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="H449" s="2">
+        <v>0</v>
+      </c>
+      <c r="I449" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="450" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>24</v>
+      </c>
+      <c r="B450" s="1">
+        <v>42751.725868055553</v>
+      </c>
+      <c r="C450">
+        <v>111964</v>
+      </c>
+      <c r="D450" t="s">
+        <v>876</v>
+      </c>
+      <c r="E450" t="s">
+        <v>1</v>
+      </c>
+      <c r="F450" s="2">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="G450" s="2">
+        <v>2.8472222222222222E-2</v>
+      </c>
+      <c r="H450" s="2">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="I450" t="s">
+        <v>877</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Games lichess are automatically fetched
</commit_message>
<xml_diff>
--- a/data/input/chesstempo_tactics.xlsx
+++ b/data/input/chesstempo_tactics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="912">
   <si>
     <t>969.4</t>
   </si>
@@ -2658,6 +2658,108 @@
   </si>
   <si>
     <t>1388.4 (-2.7)</t>
+  </si>
+  <si>
+    <t>1084.7</t>
+  </si>
+  <si>
+    <t>1385.9 (+1.1)</t>
+  </si>
+  <si>
+    <t>1400.8</t>
+  </si>
+  <si>
+    <t>1384.9 (+3.7)</t>
+  </si>
+  <si>
+    <t>1357.1</t>
+  </si>
+  <si>
+    <t>1381.2 (-3.8)</t>
+  </si>
+  <si>
+    <t>1231.6</t>
+  </si>
+  <si>
+    <t>1385.0 (+2.1)</t>
+  </si>
+  <si>
+    <t>1241.8</t>
+  </si>
+  <si>
+    <t>1382.9 (-4.9)</t>
+  </si>
+  <si>
+    <t>1440.3</t>
+  </si>
+  <si>
+    <t>1387.8 (+4.1)</t>
+  </si>
+  <si>
+    <t>1314.7</t>
+  </si>
+  <si>
+    <t>1383.7 (+2.8)</t>
+  </si>
+  <si>
+    <t>1543.8</t>
+  </si>
+  <si>
+    <t>1380.9 (+5.1)</t>
+  </si>
+  <si>
+    <t>1372.7</t>
+  </si>
+  <si>
+    <t>1375.8 (-3.6)</t>
+  </si>
+  <si>
+    <t>1425.7</t>
+  </si>
+  <si>
+    <t>1379.4 (+4.0)</t>
+  </si>
+  <si>
+    <t>1362.1</t>
+  </si>
+  <si>
+    <t>1375.4 (-3.7)</t>
+  </si>
+  <si>
+    <t>1379.1 (+2.6)</t>
+  </si>
+  <si>
+    <t>1278.1</t>
+  </si>
+  <si>
+    <t>1376.5 (-4.5)</t>
+  </si>
+  <si>
+    <t>1221.5</t>
+  </si>
+  <si>
+    <t>1381.0 (+2.0)</t>
+  </si>
+  <si>
+    <t>1149.8</t>
+  </si>
+  <si>
+    <t>1379.0 (-5.6)</t>
+  </si>
+  <si>
+    <t>1344.4</t>
+  </si>
+  <si>
+    <t>1384.5 (+3.1)</t>
+  </si>
+  <si>
+    <t>1473.0</t>
+  </si>
+  <si>
+    <t>1381.4 (-2.6)</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -2977,10 +3079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I450"/>
+  <dimension ref="A1:I468"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A410" workbookViewId="0">
-      <selection activeCell="A427" sqref="A427:I450"/>
+    <sheetView tabSelected="1" topLeftCell="A467" workbookViewId="0">
+      <selection activeCell="A468" sqref="A468:I468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16038,6 +16140,528 @@
         <v>877</v>
       </c>
     </row>
+    <row r="451" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A451">
+        <v>1</v>
+      </c>
+      <c r="B451" s="1">
+        <v>42751.804791666669</v>
+      </c>
+      <c r="C451">
+        <v>62646</v>
+      </c>
+      <c r="D451" t="s">
+        <v>878</v>
+      </c>
+      <c r="E451" t="s">
+        <v>1</v>
+      </c>
+      <c r="F451" s="2">
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="G451" s="2">
+        <v>2.5694444444444447E-2</v>
+      </c>
+      <c r="H451" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I451" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="452" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A452">
+        <v>2</v>
+      </c>
+      <c r="B452" s="1">
+        <v>42751.80431712963</v>
+      </c>
+      <c r="C452">
+        <v>171130</v>
+      </c>
+      <c r="D452" t="s">
+        <v>880</v>
+      </c>
+      <c r="E452" t="s">
+        <v>1</v>
+      </c>
+      <c r="F452" s="2">
+        <v>0.1173611111111111</v>
+      </c>
+      <c r="G452" s="2">
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="H452" s="2">
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="I452" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="453" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A453">
+        <v>3</v>
+      </c>
+      <c r="B453" s="1">
+        <v>42751.802488425928</v>
+      </c>
+      <c r="C453">
+        <v>72839</v>
+      </c>
+      <c r="D453" t="s">
+        <v>882</v>
+      </c>
+      <c r="E453" t="s">
+        <v>1</v>
+      </c>
+      <c r="F453" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G453" s="2">
+        <v>2.5694444444444447E-2</v>
+      </c>
+      <c r="H453" s="2">
+        <v>0</v>
+      </c>
+      <c r="I453" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="454" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A454">
+        <v>4</v>
+      </c>
+      <c r="B454" s="1">
+        <v>42751.80201388889</v>
+      </c>
+      <c r="C454">
+        <v>165054</v>
+      </c>
+      <c r="D454" t="s">
+        <v>884</v>
+      </c>
+      <c r="E454" t="s">
+        <v>1</v>
+      </c>
+      <c r="F454" s="2">
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="G454" s="2">
+        <v>6.458333333333334E-2</v>
+      </c>
+      <c r="H454" s="2">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="I454" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="455" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A455">
+        <v>5</v>
+      </c>
+      <c r="B455" s="1">
+        <v>42751.80060185185</v>
+      </c>
+      <c r="C455">
+        <v>101515</v>
+      </c>
+      <c r="D455" t="s">
+        <v>886</v>
+      </c>
+      <c r="E455" t="s">
+        <v>1</v>
+      </c>
+      <c r="F455" s="2">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="G455" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H455" s="2">
+        <v>0</v>
+      </c>
+      <c r="I455" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="456" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>6</v>
+      </c>
+      <c r="B456" s="1">
+        <v>42751.800208333334</v>
+      </c>
+      <c r="C456">
+        <v>98300</v>
+      </c>
+      <c r="D456" t="s">
+        <v>888</v>
+      </c>
+      <c r="E456" t="s">
+        <v>1</v>
+      </c>
+      <c r="F456" s="2">
+        <v>0.17361111111111113</v>
+      </c>
+      <c r="G456" s="2">
+        <v>0.24236111111111111</v>
+      </c>
+      <c r="H456" s="2">
+        <v>0.23541666666666669</v>
+      </c>
+      <c r="I456" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="457" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A457">
+        <v>7</v>
+      </c>
+      <c r="B457" s="1">
+        <v>42751.795324074075</v>
+      </c>
+      <c r="C457">
+        <v>130419</v>
+      </c>
+      <c r="D457" t="s">
+        <v>890</v>
+      </c>
+      <c r="E457" t="s">
+        <v>1</v>
+      </c>
+      <c r="F457" s="2">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="G457" s="2">
+        <v>0.14722222222222223</v>
+      </c>
+      <c r="H457" s="2">
+        <v>4.0972222222222222E-2</v>
+      </c>
+      <c r="I457" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="458" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A458">
+        <v>8</v>
+      </c>
+      <c r="B458" s="1">
+        <v>42751.79277777778</v>
+      </c>
+      <c r="C458">
+        <v>176365</v>
+      </c>
+      <c r="D458" t="s">
+        <v>892</v>
+      </c>
+      <c r="E458" t="s">
+        <v>1</v>
+      </c>
+      <c r="F458" s="2">
+        <v>0.2076388888888889</v>
+      </c>
+      <c r="G458" s="2">
+        <v>6.5277777777777782E-2</v>
+      </c>
+      <c r="H458" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I458" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="459" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A459">
+        <v>9</v>
+      </c>
+      <c r="B459" s="1">
+        <v>42751.791631944441</v>
+      </c>
+      <c r="C459">
+        <v>98281</v>
+      </c>
+      <c r="D459" t="s">
+        <v>894</v>
+      </c>
+      <c r="E459" t="s">
+        <v>1</v>
+      </c>
+      <c r="F459" s="2">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="G459" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H459" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="I459" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="460" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A460">
+        <v>10</v>
+      </c>
+      <c r="B460" s="1">
+        <v>42751.791331018518</v>
+      </c>
+      <c r="C460">
+        <v>88686</v>
+      </c>
+      <c r="D460" t="s">
+        <v>896</v>
+      </c>
+      <c r="E460" t="s">
+        <v>1</v>
+      </c>
+      <c r="F460" s="2">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G460" s="2">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="H460" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I460" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="461" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A461">
+        <v>11</v>
+      </c>
+      <c r="B461" s="1">
+        <v>42751.790532407409</v>
+      </c>
+      <c r="C461">
+        <v>94723</v>
+      </c>
+      <c r="D461" t="s">
+        <v>898</v>
+      </c>
+      <c r="E461" t="s">
+        <v>1</v>
+      </c>
+      <c r="F461" s="2">
+        <v>7.4305555555555555E-2</v>
+      </c>
+      <c r="G461" s="2">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="H461" s="2">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="I461" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="462" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A462">
+        <v>12</v>
+      </c>
+      <c r="B462" s="1">
+        <v>42751.789375</v>
+      </c>
+      <c r="C462">
+        <v>93001</v>
+      </c>
+      <c r="D462" t="s">
+        <v>708</v>
+      </c>
+      <c r="E462" t="s">
+        <v>1</v>
+      </c>
+      <c r="F462" s="2">
+        <v>4.3750000000000004E-2</v>
+      </c>
+      <c r="G462" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="H462" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="I462" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="463" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A463">
+        <v>13</v>
+      </c>
+      <c r="B463" s="1">
+        <v>42751.788645833331</v>
+      </c>
+      <c r="C463">
+        <v>9561</v>
+      </c>
+      <c r="D463" t="s">
+        <v>901</v>
+      </c>
+      <c r="E463" t="s">
+        <v>1</v>
+      </c>
+      <c r="F463" s="2">
+        <v>6.805555555555555E-2</v>
+      </c>
+      <c r="G463" s="2">
+        <v>0.1277777777777778</v>
+      </c>
+      <c r="H463" s="2">
+        <v>0</v>
+      </c>
+      <c r="I463" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="464" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A464">
+        <v>14</v>
+      </c>
+      <c r="B464" s="1">
+        <v>42751.786469907405</v>
+      </c>
+      <c r="C464">
+        <v>168516</v>
+      </c>
+      <c r="D464" t="s">
+        <v>903</v>
+      </c>
+      <c r="E464" t="s">
+        <v>1</v>
+      </c>
+      <c r="F464" s="2">
+        <v>9.7916666666666666E-2</v>
+      </c>
+      <c r="G464" s="2">
+        <v>6.3194444444444442E-2</v>
+      </c>
+      <c r="H464" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I464" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="465" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A465">
+        <v>15</v>
+      </c>
+      <c r="B465" s="1">
+        <v>42751.785312499997</v>
+      </c>
+      <c r="C465">
+        <v>60487</v>
+      </c>
+      <c r="D465" t="s">
+        <v>905</v>
+      </c>
+      <c r="E465" t="s">
+        <v>1</v>
+      </c>
+      <c r="F465" s="2">
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="G465" s="2">
+        <v>2.5694444444444447E-2</v>
+      </c>
+      <c r="H465" s="2">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="I465" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="466" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A466">
+        <v>16</v>
+      </c>
+      <c r="B466" s="1">
+        <v>42751.784479166665</v>
+      </c>
+      <c r="C466">
+        <v>59164</v>
+      </c>
+      <c r="D466" t="s">
+        <v>907</v>
+      </c>
+      <c r="E466" t="s">
+        <v>1</v>
+      </c>
+      <c r="F466" s="2">
+        <v>5.1388888888888894E-2</v>
+      </c>
+      <c r="G466" s="2">
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="H466" s="2">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="I466" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="467" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A467">
+        <v>17</v>
+      </c>
+      <c r="B467" s="1">
+        <v>42751.783935185187</v>
+      </c>
+      <c r="C467">
+        <v>171359</v>
+      </c>
+      <c r="D467" t="s">
+        <v>909</v>
+      </c>
+      <c r="E467" t="s">
+        <v>1</v>
+      </c>
+      <c r="F467" s="2">
+        <v>0.20069444444444443</v>
+      </c>
+      <c r="G467" s="2">
+        <v>8.5416666666666655E-2</v>
+      </c>
+      <c r="H467" s="2">
+        <v>0</v>
+      </c>
+      <c r="I467" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="468" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>911</v>
+      </c>
+      <c r="B468" t="s">
+        <v>911</v>
+      </c>
+      <c r="C468" t="s">
+        <v>911</v>
+      </c>
+      <c r="D468" t="s">
+        <v>911</v>
+      </c>
+      <c r="E468" t="s">
+        <v>911</v>
+      </c>
+      <c r="F468" t="s">
+        <v>911</v>
+      </c>
+      <c r="G468" t="s">
+        <v>911</v>
+      </c>
+      <c r="H468" t="s">
+        <v>911</v>
+      </c>
+      <c r="I468" t="s">
+        <v>911</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>